<commit_message>
Updated project link in documentation files.
</commit_message>
<xml_diff>
--- a/doc/instance-expiration-cost-estimate.xlsx
+++ b/doc/instance-expiration-cost-estimate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\Cdk\ec2-instance-watchdog\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\guidance-for-instance-expiration-on-aws\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D0C743D-23F4-4DAC-9366-684E94B79FD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AB2AFB1-C5E1-4610-93EC-55A6584BB9B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E24FE04E-2BAD-469E-9CCD-04368567B0DD}"/>
+    <workbookView xWindow="33615" yWindow="8685" windowWidth="21600" windowHeight="11235" xr2:uid="{E24FE04E-2BAD-469E-9CCD-04368567B0DD}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" r:id="rId1"/>
@@ -2173,7 +2173,7 @@
     <hyperlink ref="F37" r:id="rId2" xr:uid="{3697308E-3076-4C67-8C3D-E99C899438A6}"/>
     <hyperlink ref="F47" r:id="rId3" xr:uid="{3A311B74-9A92-4717-8637-3F3E0DA5E1E7}"/>
     <hyperlink ref="F54" r:id="rId4" xr:uid="{FA75757F-7913-48D0-A10E-B9651A4E639D}"/>
-    <hyperlink ref="C7" r:id="rId5" display="EC2 Instance Watchdog" xr:uid="{2299A522-9AF8-48BC-AEDC-A351890C04DA}"/>
+    <hyperlink ref="C7" r:id="rId5" xr:uid="{2299A522-9AF8-48BC-AEDC-A351890C04DA}"/>
     <hyperlink ref="F62" r:id="rId6" xr:uid="{96EC9F8D-5927-47A2-A4F3-439886265821}"/>
     <hyperlink ref="F68" r:id="rId7" xr:uid="{C5182291-0C1B-4F67-9F05-2D27FC27E1FA}"/>
     <hyperlink ref="F73" r:id="rId8" xr:uid="{D67C9753-4982-4312-8F22-C055C7A5BC89}"/>

</xml_diff>